<commit_message>
Update of Python script for the bootstrapped evaluation metrics
</commit_message>
<xml_diff>
--- a/evaluation/COCA_web_5080941.xlsx
+++ b/evaluation/COCA_web_5080941.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE3E60D-77A7-5540-AF72-0DF37550FB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D9AF35-A045-C042-9484-D064263D098A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EBDBF9A0-63DD-2448-B125-968A97D2DE8E}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="653">
   <si>
     <t>October</t>
   </si>
@@ -2387,8 +2387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F7E882-C8E9-3844-9BCF-1429478D5DED}">
   <dimension ref="A1:H675"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="159" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6721,7 +6721,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>528</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>529</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>530</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>531</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>337</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>508</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>366</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>439</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>527</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>532</v>
       </c>
@@ -6836,11 +6836,8 @@
       <c r="F394" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="H394" s="3" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>484</v>
       </c>
@@ -6851,7 +6848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>533</v>
       </c>
@@ -6862,7 +6859,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>337</v>
       </c>
@@ -6873,7 +6870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>534</v>
       </c>
@@ -6884,7 +6881,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>450</v>
       </c>
@@ -6895,7 +6892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>450</v>
       </c>
@@ -7082,7 +7079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>337</v>
       </c>
@@ -7093,7 +7090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>538</v>
       </c>
@@ -7104,7 +7101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>539</v>
       </c>
@@ -7115,7 +7112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>365</v>
       </c>
@@ -7126,7 +7123,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>366</v>
       </c>
@@ -7137,7 +7134,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>509</v>
       </c>
@@ -7148,7 +7145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>482</v>
       </c>
@@ -7162,7 +7159,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>540</v>
       </c>
@@ -7173,7 +7170,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>484</v>
       </c>
@@ -7184,7 +7181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>541</v>
       </c>
@@ -7195,7 +7192,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>542</v>
       </c>
@@ -7208,11 +7205,8 @@
       <c r="F427" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="H427" s="3" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>543</v>
       </c>
@@ -7223,7 +7217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>373</v>
       </c>
@@ -7234,7 +7228,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>374</v>
       </c>
@@ -7245,7 +7239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>407</v>
       </c>
@@ -7261,11 +7255,8 @@
       <c r="F431" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="H431" s="3" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>505</v>
       </c>
@@ -7631,7 +7622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>371</v>
       </c>
@@ -7642,7 +7633,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>559</v>
       </c>
@@ -7653,7 +7644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>370</v>
       </c>
@@ -7664,7 +7655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>360</v>
       </c>
@@ -7675,7 +7666,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>405</v>
       </c>
@@ -7686,7 +7677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="470" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>349</v>
       </c>
@@ -7697,7 +7688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>560</v>
       </c>
@@ -7708,7 +7699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>538</v>
       </c>
@@ -7719,7 +7710,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="473" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>561</v>
       </c>
@@ -7730,7 +7721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>343</v>
       </c>
@@ -7743,11 +7734,8 @@
       <c r="F474" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H474" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>332</v>
       </c>
@@ -7758,7 +7746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>562</v>
       </c>
@@ -7769,7 +7757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>366</v>
       </c>
@@ -7780,7 +7768,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="478" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>563</v>
       </c>
@@ -7791,7 +7779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>564</v>
       </c>
@@ -7805,7 +7793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>430</v>
       </c>
@@ -8356,7 +8344,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="529" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>586</v>
       </c>
@@ -8367,7 +8355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="530" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>405</v>
       </c>
@@ -8378,7 +8366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="531" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>484</v>
       </c>
@@ -8389,7 +8377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="532" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>587</v>
       </c>
@@ -8400,7 +8388,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="533" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>411</v>
       </c>
@@ -8411,7 +8399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="534" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>588</v>
       </c>
@@ -8425,7 +8413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="535" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>589</v>
       </c>
@@ -8436,7 +8424,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="536" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>405</v>
       </c>
@@ -8447,7 +8435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="537" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>349</v>
       </c>
@@ -8458,7 +8446,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="538" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>590</v>
       </c>
@@ -8469,7 +8457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="539" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>591</v>
       </c>
@@ -8483,7 +8471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="540" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>504</v>
       </c>
@@ -8496,11 +8484,8 @@
       <c r="F540" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H540" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="541" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>592</v>
       </c>
@@ -8511,7 +8496,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="542" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>337</v>
       </c>
@@ -8522,7 +8507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="543" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>593</v>
       </c>
@@ -8533,7 +8518,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="544" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>594</v>
       </c>

</xml_diff>